<commit_message>
Release TUM Lite 2.3 & TUM Enchanted 1.4
</commit_message>
<xml_diff>
--- a/TUM Lite Enchanted/Data/s/-100 Neutral Towns guards accumulation.xlsx
+++ b/TUM Lite Enchanted/Data/s/-100 Neutral Towns guards accumulation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Heroes of Might And Magic 3 ERA\Mods\MyMods TUM Lite Enchanted\Data\s\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Heroes of Might And Magic 3 ERA\Repository\TUM Lite Enchanted\Data\s\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Fine 1 mese</t>
   </si>
@@ -59,9 +59,6 @@
     <t>1/2/1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>2-4</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>3 lvl 1-2-3-4-5</t>
-  </si>
-  <si>
-    <t>3 lvl 6-7</t>
   </si>
   <si>
     <t>2/4/1</t>
@@ -162,6 +156,33 @@
   </si>
   <si>
     <t>*15/45 for Castle &amp; Rampart</t>
+  </si>
+  <si>
+    <t>3 lvl 6</t>
+  </si>
+  <si>
+    <t>3 lvl 7</t>
+  </si>
+  <si>
+    <t>3/3/1</t>
+  </si>
+  <si>
+    <t>3/4/1</t>
+  </si>
+  <si>
+    <t>4/1/1</t>
+  </si>
+  <si>
+    <t>3*</t>
+  </si>
+  <si>
+    <t>* = 5% chance to get 3 lvl6 units instead of the rolls</t>
+  </si>
+  <si>
+    <t>MONTH 4+</t>
+  </si>
+  <si>
+    <t>1*(Month 2)</t>
   </si>
 </sst>
 </file>
@@ -185,12 +206,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -205,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,10 +259,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -521,7 +568,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,23 +584,26 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
+      <c r="E2" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
@@ -574,11 +624,14 @@
         <f t="shared" ref="C3:C9" si="0">(K3-I3)/4</f>
         <v>65</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
+      <c r="D3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
       </c>
       <c r="I3" s="3">
         <v>80</v>
@@ -600,7 +653,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="14"/>
       <c r="I4" s="3">
         <v>40</v>
       </c>
@@ -621,7 +675,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="14"/>
       <c r="I5" s="3">
         <v>16</v>
       </c>
@@ -642,7 +697,8 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="14"/>
       <c r="I6" s="3">
         <v>9</v>
       </c>
@@ -663,7 +719,8 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="14"/>
       <c r="I7" s="3">
         <v>6</v>
       </c>
@@ -684,7 +741,8 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="14"/>
       <c r="I8" s="3">
         <v>4</v>
       </c>
@@ -705,7 +763,8 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="14"/>
       <c r="I9" s="3">
         <v>1</v>
       </c>
@@ -716,25 +775,25 @@
     </row>
     <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="F11" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H11" s="7"/>
     </row>
@@ -745,73 +804,76 @@
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
+      <c r="C12" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
+      <c r="I12" s="16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>31</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -821,18 +883,18 @@
         <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="6"/>
     </row>
@@ -841,22 +903,22 @@
         <v>3</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G17" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="6"/>
     </row>
@@ -865,43 +927,43 @@
         <v>4</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -911,16 +973,16 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>25</v>
+      <c r="D20" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H20" s="6"/>
     </row>
@@ -929,38 +991,55 @@
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
-        <v>25</v>
+      <c r="D21" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="6" t="s">
-        <v>22</v>
+      <c r="G21" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
+      <c r="D23" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
+      <c r="D24" s="13">
+        <v>2</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
@@ -976,9 +1055,10 @@
       <c r="A31" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D3:D9"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E3:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>